<commit_message>
Atualizacao da Base de Dados dos Pacientes Encaminhados
</commit_message>
<xml_diff>
--- a/pacientes_imuno_mediados_encaminhados_27_02-2024.xlsx
+++ b/pacientes_imuno_mediados_encaminhados_27_02-2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keller\Documents\Projetos\Cursos\Python\Dashboard_Area_Logada\Area_Logada\venv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keller\Documents\Projetos\Cursos\Python\Dashboard_Area_Logada\Area_Logada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B513DBA8-6C48-4230-95F6-B1181FB3FF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D3B019-634E-4A1F-B803-7478EBE4AF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Encaminhamento Imuno" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="172">
   <si>
     <t>Número do caso</t>
   </si>
@@ -527,6 +527,15 @@
   </si>
   <si>
     <t>Quantidade</t>
+  </si>
+  <si>
+    <t>00879757</t>
+  </si>
+  <si>
+    <t>ALMERINDA ROCHA SILVA</t>
+  </si>
+  <si>
+    <t>07/03/2024 10:09</t>
   </si>
 </sst>
 </file>
@@ -618,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -641,16 +650,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -967,26 +967,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="4" width="49.85546875" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" style="4" customWidth="1"/>
     <col min="6" max="6" width="29.85546875" customWidth="1"/>
     <col min="7" max="7" width="40.140625" customWidth="1"/>
     <col min="8" max="8" width="18.140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -998,7 +998,7 @@
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="3" t="s">
         <v>164</v>
       </c>
       <c r="F1" s="6" t="s">
@@ -1012,71 +1012,71 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="7">
+        <v>26191</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E3" s="7">
         <v>34799</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="9">
-        <v>750352</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>750352</v>
       </c>
       <c r="F4" s="7" t="s">
@@ -1090,149 +1090,149 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="7">
+        <v>750352</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E6" s="7">
         <v>135992</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E7" s="7">
         <v>47505</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E8" s="7">
         <v>19869</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F8" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E9" s="7">
         <v>750352</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="9">
-        <v>34799</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="9">
+      <c r="E10" s="7">
         <v>34799</v>
       </c>
       <c r="F10" s="7" t="s">
@@ -1246,19 +1246,19 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>41</v>
+      <c r="A11" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="7">
         <v>34799</v>
       </c>
       <c r="F11" s="7" t="s">
@@ -1272,253 +1272,253 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="7">
+        <v>34799</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E13" s="7">
         <v>135992</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="H13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E14" s="7">
         <v>58475</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E15" s="7">
         <v>8157</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="H15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E16" s="7">
         <v>99999</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H15" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="H16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E17" s="7">
         <v>135992</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="H17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E18" s="7">
         <v>26191</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F18" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H17" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="H18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E19" s="7">
         <v>9236</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F19" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H18" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="H19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E20" s="7">
         <v>58475</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F20" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H19" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="H20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="9">
-        <v>19869</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="7">
         <v>19869</v>
       </c>
       <c r="F21" s="7" t="s">
@@ -1532,149 +1532,149 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="7">
+        <v>19869</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E23" s="7">
         <v>135992</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="H23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E24" s="7">
         <v>30024</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F24" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H23" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="H24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E25" s="7">
         <v>37001</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F25" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H24" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="H25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E26" s="7">
         <v>9236</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F26" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H25" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="H26" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E26" s="9">
-        <v>135992</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="9">
+      <c r="E27" s="7">
         <v>135992</v>
       </c>
       <c r="F27" s="7" t="s">
@@ -1688,71 +1688,71 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>105</v>
+      <c r="A28" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="9">
-        <v>9939969</v>
+      <c r="E28" s="7">
+        <v>135992</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>158</v>
       </c>
       <c r="G28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="7">
+        <v>9939969</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H28" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="H29" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="9">
-        <v>750352</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="7">
         <v>750352</v>
       </c>
       <c r="F30" s="7" t="s">
@@ -1766,19 +1766,19 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>115</v>
+      <c r="A31" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="7">
         <v>750352</v>
       </c>
       <c r="F31" s="7" t="s">
@@ -1792,19 +1792,19 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>118</v>
+      <c r="A32" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="7">
         <v>750352</v>
       </c>
       <c r="F32" s="7" t="s">
@@ -1818,19 +1818,19 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>121</v>
+      <c r="A33" s="7" t="s">
+        <v>118</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="7">
         <v>750352</v>
       </c>
       <c r="F33" s="7" t="s">
@@ -1844,45 +1844,45 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="7">
+        <v>750352</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E34" s="9">
-        <v>19869</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H34" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="7">
         <v>19869</v>
       </c>
       <c r="F35" s="7" t="s">
@@ -1896,19 +1896,19 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>130</v>
+      <c r="A36" s="7" t="s">
+        <v>127</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="7">
         <v>19869</v>
       </c>
       <c r="F36" s="7" t="s">
@@ -1922,123 +1922,123 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>133</v>
+      <c r="A37" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E37" s="9">
-        <v>37001</v>
+        <v>29</v>
+      </c>
+      <c r="E37" s="7">
+        <v>19869</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>159</v>
       </c>
       <c r="G37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="7">
+        <v>37001</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H37" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+      <c r="H38" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E39" s="7">
         <v>9236</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F39" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H38" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="H39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E40" s="7">
         <v>55450</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F40" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="H39" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="H40" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E40" s="9">
-        <v>37001</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H40" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E41" s="9">
+      <c r="E41" s="7">
         <v>37001</v>
       </c>
       <c r="F41" s="7" t="s">
@@ -2052,54 +2052,80 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="7">
+        <v>37001</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H42" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E42" s="9">
+      <c r="E43" s="7">
         <v>55450</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F43" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="H42" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
+      <c r="H43" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E43" s="9">
+      <c r="E44" s="7">
         <v>750352</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="F44" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H43" s="4">
+      <c r="H44" s="4">
         <v>1</v>
       </c>
     </row>
@@ -2107,7 +2133,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:A3 A4:A43" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:A4 A5:A44" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizacao Base de Dados Pacientes Encaminhados
</commit_message>
<xml_diff>
--- a/pacientes_imuno_mediados_encaminhados_27_02-2024.xlsx
+++ b/pacientes_imuno_mediados_encaminhados_27_02-2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keller\Documents\Projetos\Cursos\Python\Dashboard_Area_Logada\Area_Logada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D909CCB-EC35-4829-8C15-2DC687E3AF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B3F4CB-8325-4506-9FF7-195A4F3A6390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Encaminhamento Imuno" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="184">
   <si>
     <t>Número do caso</t>
   </si>
@@ -554,13 +554,31 @@
   </si>
   <si>
     <t>12/03/2024 13:38</t>
+  </si>
+  <si>
+    <t>00907436</t>
+  </si>
+  <si>
+    <t>Larissa de Oliveira Pereira Fonseca Monlevad</t>
+  </si>
+  <si>
+    <t>19/03/2024 12:35</t>
+  </si>
+  <si>
+    <t>00908845</t>
+  </si>
+  <si>
+    <t>Ingrid Rolim Mendes Araujo</t>
+  </si>
+  <si>
+    <t>19/03/2024 16:54</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -605,6 +623,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF56585B"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF56585B"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -655,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -678,8 +702,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -691,7 +714,11 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1008,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,157 +1079,157 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="14">
+        <v>135992</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="14">
+        <v>750352</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E4" s="7">
         <v>750352</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="H4" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E5" s="6">
         <v>19869</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="6">
-        <v>26191</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="6">
-        <v>34799</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="H5" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>7</v>
+        <v>169</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>171</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E6" s="6">
-        <v>750352</v>
+        <v>26191</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="4">
+        <v>69</v>
+      </c>
+      <c r="H6" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>12</v>
+      <c r="A7" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E7" s="6">
-        <v>750352</v>
+        <v>34799</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H7" s="4">
         <v>1</v>
@@ -1210,25 +1237,25 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E8" s="6">
-        <v>135992</v>
+        <v>750352</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H8" s="4">
         <v>1</v>
@@ -1236,25 +1263,25 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E9" s="6">
-        <v>47505</v>
+        <v>750352</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="H9" s="4">
         <v>1</v>
@@ -1262,25 +1289,25 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E10" s="6">
-        <v>19869</v>
+        <v>135992</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H10" s="4">
         <v>1</v>
@@ -1288,25 +1315,25 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E11" s="6">
-        <v>750352</v>
+        <v>47505</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="H11" s="4">
         <v>1</v>
@@ -1314,25 +1341,25 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E12" s="6">
-        <v>34799</v>
+        <v>19869</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="H12" s="4">
         <v>1</v>
@@ -1340,25 +1367,25 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E13" s="6">
-        <v>34799</v>
+        <v>750352</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H13" s="4">
         <v>1</v>
@@ -1366,16 +1393,16 @@
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="E14" s="6">
         <v>34799</v>
@@ -1392,25 +1419,25 @@
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E15" s="6">
-        <v>135992</v>
+        <v>34799</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="H15" s="4">
         <v>1</v>
@@ -1418,25 +1445,25 @@
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E16" s="6">
-        <v>58475</v>
+        <v>34799</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>156</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="H16" s="4">
         <v>1</v>
@@ -1444,25 +1471,25 @@
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E17" s="6">
-        <v>8157</v>
+        <v>135992</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="H17" s="4">
         <v>1</v>
@@ -1470,25 +1497,25 @@
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E18" s="6">
-        <v>99999</v>
+        <v>58475</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="H18" s="4">
         <v>1</v>
@@ -1496,25 +1523,25 @@
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="E19" s="6">
-        <v>135992</v>
+        <v>8157</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="H19" s="4">
         <v>1</v>
@@ -1522,25 +1549,25 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E20" s="6">
-        <v>26191</v>
+        <v>99999</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="H20" s="4">
         <v>1</v>
@@ -1548,25 +1575,25 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>163</v>
+        <v>19</v>
       </c>
       <c r="E21" s="6">
-        <v>9236</v>
+        <v>135992</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="H21" s="4">
         <v>1</v>
@@ -1574,25 +1601,25 @@
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="E22" s="6">
-        <v>58475</v>
+        <v>26191</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="H22" s="4">
         <v>1</v>
@@ -1600,25 +1627,25 @@
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>29</v>
+        <v>163</v>
       </c>
       <c r="E23" s="6">
-        <v>19869</v>
+        <v>9236</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="H23" s="4">
         <v>1</v>
@@ -1626,25 +1653,25 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="E24" s="6">
-        <v>19869</v>
+        <v>58475</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="H24" s="4">
         <v>1</v>
@@ -1652,25 +1679,25 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E25" s="6">
-        <v>135992</v>
+        <v>19869</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H25" s="4">
         <v>1</v>
@@ -1678,25 +1705,25 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="E26" s="6">
-        <v>30024</v>
+        <v>19869</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="H26" s="4">
         <v>1</v>
@@ -1704,25 +1731,25 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E27" s="6">
-        <v>37001</v>
+        <v>135992</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="H27" s="4">
         <v>1</v>
@@ -1730,25 +1757,25 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>163</v>
+        <v>89</v>
       </c>
       <c r="E28" s="6">
-        <v>9236</v>
+        <v>30024</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="H28" s="4">
         <v>1</v>
@@ -1756,25 +1783,25 @@
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>101</v>
+        <v>29</v>
       </c>
       <c r="E29" s="6">
-        <v>135992</v>
+        <v>37001</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="H29" s="4">
         <v>1</v>
@@ -1782,25 +1809,25 @@
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>19</v>
+        <v>163</v>
       </c>
       <c r="E30" s="6">
-        <v>135992</v>
+        <v>9236</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="H30" s="4">
         <v>1</v>
@@ -1808,25 +1835,25 @@
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="E31" s="6">
-        <v>9939969</v>
+        <v>135992</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>158</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>108</v>
+        <v>20</v>
       </c>
       <c r="H31" s="4">
         <v>1</v>
@@ -1834,25 +1861,25 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E32" s="6">
-        <v>750352</v>
+        <v>135992</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H32" s="4">
         <v>1</v>
@@ -1860,25 +1887,25 @@
     </row>
     <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E33" s="6">
-        <v>750352</v>
+        <v>9939969</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>11</v>
+        <v>108</v>
       </c>
       <c r="H33" s="4">
         <v>1</v>
@@ -1886,13 +1913,13 @@
     </row>
     <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>10</v>
@@ -1912,13 +1939,13 @@
     </row>
     <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>10</v>
@@ -1938,13 +1965,13 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>10</v>
@@ -1964,25 +1991,25 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E37" s="6">
-        <v>19869</v>
+        <v>750352</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H37" s="4">
         <v>1</v>
@@ -1990,25 +2017,25 @@
     </row>
     <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E38" s="6">
-        <v>19869</v>
+        <v>750352</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H38" s="4">
         <v>1</v>
@@ -2016,13 +2043,13 @@
     </row>
     <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>29</v>
@@ -2042,25 +2069,25 @@
     </row>
     <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E40" s="6">
-        <v>37001</v>
+        <v>19869</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>159</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="H40" s="4">
         <v>1</v>
@@ -2068,25 +2095,25 @@
     </row>
     <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>163</v>
+        <v>29</v>
       </c>
       <c r="E41" s="6">
-        <v>9236</v>
+        <v>19869</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="H41" s="4">
         <v>1</v>
@@ -2094,25 +2121,25 @@
     </row>
     <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="E42" s="6">
-        <v>55450</v>
+        <v>37001</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="H42" s="4">
         <v>1</v>
@@ -2120,25 +2147,25 @@
     </row>
     <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>19</v>
+        <v>163</v>
       </c>
       <c r="E43" s="6">
-        <v>37001</v>
+        <v>9236</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H43" s="4">
         <v>1</v>
@@ -2146,25 +2173,25 @@
     </row>
     <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="E44" s="6">
-        <v>37001</v>
+        <v>55450</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
       <c r="H44" s="4">
         <v>1</v>
@@ -2172,25 +2199,25 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="E45" s="6">
-        <v>55450</v>
+        <v>37001</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="H45" s="4">
         <v>1</v>
@@ -2198,27 +2225,79 @@
     </row>
     <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" s="6">
+        <v>37001</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H46" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" s="6">
+        <v>55450</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H47" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E48" s="6">
         <v>750352</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="F48" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H46" s="4">
+      <c r="H48" s="4">
         <v>1</v>
       </c>
     </row>
@@ -2226,7 +2305,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:A6 A7:A46" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:A8 A9:A48" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizacao da Relacao dos Pacientes Encaminhados ate o dia 16/04/2024
</commit_message>
<xml_diff>
--- a/pacientes_imuno_mediados_encaminhados_27_02-2024.xlsx
+++ b/pacientes_imuno_mediados_encaminhados_27_02-2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keller\Documents\Projetos\Cursos\Python\Dashboard_Area_Logada\Area_Logada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B2B9A4-BD0F-4E79-9D47-7702380E1CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13ACD378-69E0-4B4C-9658-B484AB2C940E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Encaminhamento Imuno" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="225">
   <si>
     <t>Número do caso</t>
   </si>
@@ -659,6 +659,42 @@
   </si>
   <si>
     <t>05/04/2024 17:54</t>
+  </si>
+  <si>
+    <t>00963230</t>
+  </si>
+  <si>
+    <t>00956562</t>
+  </si>
+  <si>
+    <t>CARMEN LUCIA FERNANDES</t>
+  </si>
+  <si>
+    <t>10/04/2024 10:35</t>
+  </si>
+  <si>
+    <t>OC ONCOCLÍNICAS ARAGUARI</t>
+  </si>
+  <si>
+    <t>Gustavo Pafume de Sa</t>
+  </si>
+  <si>
+    <t>Maria Dulce Pereira Rodrigues</t>
+  </si>
+  <si>
+    <t>12/04/2024 15:15</t>
+  </si>
+  <si>
+    <t>00966970</t>
+  </si>
+  <si>
+    <t>Celia Teixeira Andrade</t>
+  </si>
+  <si>
+    <t>15/04/2024 17:11</t>
+  </si>
+  <si>
+    <t>Renato de Lima Azambuja</t>
   </si>
 </sst>
 </file>
@@ -806,20 +842,18 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1134,10 +1168,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,226 +1214,226 @@
     </row>
     <row r="2" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E2" s="7">
-        <v>135992</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>158</v>
+        <v>849960</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>157</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="15">
+        <v>224</v>
+      </c>
+      <c r="H2" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="7">
+        <v>68688</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="E4" s="7">
+        <v>68688</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="H4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="7">
+        <v>135992</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B6" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E6" s="7">
         <v>6776</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F6" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="H3" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="H6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B7" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E7" s="7">
         <v>10218</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F7" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G7" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="H4" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B8" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E8" s="7">
         <v>9236</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F8" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="H5" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B9" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E9" s="7">
         <v>750352</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F9" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="H9" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B10" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="7">
-        <v>750352</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="E8" s="15">
-        <v>158550</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="H8" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="8">
-        <v>135992</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>750352</v>
       </c>
       <c r="F10" s="8" t="s">
@@ -1414,181 +1448,181 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>176</v>
+        <v>188</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>184</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="7">
-        <v>750352</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>157</v>
+        <v>186</v>
+      </c>
+      <c r="E11" s="8">
+        <v>158550</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>158</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="17">
+        <v>187</v>
+      </c>
+      <c r="H11" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="6">
-        <v>19869</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>159</v>
+      <c r="A12" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="8">
+        <v>135992</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>158</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="17">
+        <v>20</v>
+      </c>
+      <c r="H12" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="6">
-        <v>26191</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H13" s="11">
+        <v>15</v>
+      </c>
+      <c r="E13" s="8">
+        <v>750352</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="6">
-        <v>34799</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="4">
+        <v>175</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="7">
+        <v>750352</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>7</v>
+        <v>172</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>173</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>9</v>
+        <v>174</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E15" s="6">
-        <v>750352</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="4">
+        <v>19869</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>12</v>
+        <v>169</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>14</v>
+        <v>171</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="E16" s="6">
-        <v>750352</v>
+        <v>26191</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="4">
+        <v>69</v>
+      </c>
+      <c r="H16" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>16</v>
+      <c r="A17" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>18</v>
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E17" s="6">
-        <v>135992</v>
+        <v>34799</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="H17" s="4">
         <v>1</v>
@@ -1596,25 +1630,25 @@
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E18" s="6">
-        <v>47505</v>
+        <v>750352</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="H18" s="4">
         <v>1</v>
@@ -1622,25 +1656,25 @@
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E19" s="6">
-        <v>19869</v>
+        <v>750352</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H19" s="4">
         <v>1</v>
@@ -1648,25 +1682,25 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E20" s="6">
-        <v>750352</v>
+        <v>135992</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H20" s="4">
         <v>1</v>
@@ -1674,25 +1708,25 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="E21" s="6">
-        <v>34799</v>
+        <v>47505</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>156</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="H21" s="4">
         <v>1</v>
@@ -1700,25 +1734,25 @@
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="E22" s="6">
-        <v>34799</v>
+        <v>19869</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="H22" s="4">
         <v>1</v>
@@ -1726,25 +1760,25 @@
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E23" s="6">
-        <v>34799</v>
+        <v>750352</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H23" s="4">
         <v>1</v>
@@ -1752,25 +1786,25 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="E24" s="6">
-        <v>135992</v>
+        <v>34799</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="H24" s="4">
         <v>1</v>
@@ -1778,25 +1812,25 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E25" s="6">
-        <v>58475</v>
+        <v>34799</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>156</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="H25" s="4">
         <v>1</v>
@@ -1804,25 +1838,25 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="E26" s="6">
-        <v>8157</v>
+        <v>34799</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="H26" s="4">
         <v>1</v>
@@ -1830,25 +1864,25 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="E27" s="6">
-        <v>99999</v>
+        <v>135992</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="H27" s="4">
         <v>1</v>
@@ -1856,25 +1890,25 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="E28" s="6">
-        <v>135992</v>
+        <v>58475</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="H28" s="4">
         <v>1</v>
@@ -1882,25 +1916,25 @@
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E29" s="6">
-        <v>26191</v>
+        <v>8157</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>160</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="H29" s="4">
         <v>1</v>
@@ -1908,25 +1942,25 @@
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>163</v>
+        <v>60</v>
       </c>
       <c r="E30" s="6">
-        <v>9236</v>
+        <v>99999</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="H30" s="4">
         <v>1</v>
@@ -1934,25 +1968,25 @@
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="E31" s="6">
-        <v>58475</v>
+        <v>135992</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H31" s="4">
         <v>1</v>
@@ -1960,25 +1994,25 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="E32" s="6">
-        <v>19869</v>
+        <v>26191</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="H32" s="4">
         <v>1</v>
@@ -1986,25 +2020,25 @@
     </row>
     <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>29</v>
+        <v>163</v>
       </c>
       <c r="E33" s="6">
-        <v>19869</v>
+        <v>9236</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="H33" s="4">
         <v>1</v>
@@ -2012,25 +2046,25 @@
     </row>
     <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="E34" s="6">
-        <v>135992</v>
+        <v>58475</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="H34" s="4">
         <v>1</v>
@@ -2038,25 +2072,25 @@
     </row>
     <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="E35" s="6">
-        <v>30024</v>
+        <v>19869</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="H35" s="4">
         <v>1</v>
@@ -2064,25 +2098,25 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E36" s="6">
-        <v>37001</v>
+        <v>19869</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>159</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="H36" s="4">
         <v>1</v>
@@ -2090,25 +2124,25 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>163</v>
+        <v>19</v>
       </c>
       <c r="E37" s="6">
-        <v>9236</v>
+        <v>135992</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="H37" s="4">
         <v>1</v>
@@ -2116,25 +2150,25 @@
     </row>
     <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="E38" s="6">
-        <v>135992</v>
+        <v>30024</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="H38" s="4">
         <v>1</v>
@@ -2142,25 +2176,25 @@
     </row>
     <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E39" s="6">
-        <v>135992</v>
+        <v>37001</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="H39" s="4">
         <v>1</v>
@@ -2168,25 +2202,25 @@
     </row>
     <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>19</v>
+        <v>163</v>
       </c>
       <c r="E40" s="6">
-        <v>9939969</v>
+        <v>9236</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="H40" s="4">
         <v>1</v>
@@ -2194,25 +2228,25 @@
     </row>
     <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="E41" s="6">
-        <v>750352</v>
+        <v>135992</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H41" s="4">
         <v>1</v>
@@ -2220,25 +2254,25 @@
     </row>
     <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E42" s="6">
-        <v>750352</v>
+        <v>135992</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H42" s="4">
         <v>1</v>
@@ -2246,25 +2280,25 @@
     </row>
     <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E43" s="6">
-        <v>750352</v>
+        <v>9939969</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>11</v>
+        <v>108</v>
       </c>
       <c r="H43" s="4">
         <v>1</v>
@@ -2272,13 +2306,13 @@
     </row>
     <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>10</v>
@@ -2298,13 +2332,13 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>10</v>
@@ -2324,25 +2358,25 @@
     </row>
     <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E46" s="6">
-        <v>19869</v>
+        <v>750352</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H46" s="4">
         <v>1</v>
@@ -2350,25 +2384,25 @@
     </row>
     <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E47" s="6">
-        <v>19869</v>
+        <v>750352</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H47" s="4">
         <v>1</v>
@@ -2376,25 +2410,25 @@
     </row>
     <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E48" s="6">
-        <v>19869</v>
+        <v>750352</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H48" s="4">
         <v>1</v>
@@ -2402,25 +2436,25 @@
     </row>
     <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E49" s="6">
-        <v>37001</v>
+        <v>19869</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>159</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="H49" s="4">
         <v>1</v>
@@ -2428,25 +2462,25 @@
     </row>
     <row r="50" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>163</v>
+        <v>29</v>
       </c>
       <c r="E50" s="6">
-        <v>9236</v>
+        <v>19869</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="H50" s="4">
         <v>1</v>
@@ -2454,25 +2488,25 @@
     </row>
     <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="E51" s="6">
-        <v>55450</v>
+        <v>19869</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>142</v>
+        <v>30</v>
       </c>
       <c r="H51" s="4">
         <v>1</v>
@@ -2480,13 +2514,13 @@
     </row>
     <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>19</v>
@@ -2506,25 +2540,25 @@
     </row>
     <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>37</v>
+        <v>163</v>
       </c>
       <c r="E53" s="6">
-        <v>37001</v>
+        <v>9236</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H53" s="4">
         <v>1</v>
@@ -2532,13 +2566,13 @@
     </row>
     <row r="54" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>50</v>
@@ -2558,27 +2592,105 @@
     </row>
     <row r="55" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="6">
+        <v>37001</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H55" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E56" s="6">
+        <v>37001</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H56" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E57" s="6">
+        <v>55450</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H57" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="6">
+      <c r="E58" s="6">
         <v>750352</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="F58" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="G58" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H55" s="4">
+      <c r="H58" s="4">
         <v>1</v>
       </c>
     </row>
@@ -2586,7 +2698,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:A15 A16:A55" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:A18 A19:A58" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizacao Relatorio Pacientes Encaminhados ate 22-04-2024
</commit_message>
<xml_diff>
--- a/pacientes_imuno_mediados_encaminhados_27_02-2024.xlsx
+++ b/pacientes_imuno_mediados_encaminhados_27_02-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keller\Documents\Projetos\Cursos\Python\Dashboard_Area_Logada\Area_Logada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13ACD378-69E0-4B4C-9658-B484AB2C940E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD57A93A-CDD5-4D9C-8C01-52BE1607C512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="237">
   <si>
     <t>Número do caso</t>
   </si>
@@ -695,6 +695,42 @@
   </si>
   <si>
     <t>Renato de Lima Azambuja</t>
+  </si>
+  <si>
+    <t>00969183</t>
+  </si>
+  <si>
+    <t>Alejandra Carolina Caceres Rigo</t>
+  </si>
+  <si>
+    <t>16/04/2024 13:30</t>
+  </si>
+  <si>
+    <t>00969757</t>
+  </si>
+  <si>
+    <t>Suelen Previdi Cortes Pugsley</t>
+  </si>
+  <si>
+    <t>16/04/2024 15:56</t>
+  </si>
+  <si>
+    <t>00971425</t>
+  </si>
+  <si>
+    <t>Rian Ibiapina Rosa</t>
+  </si>
+  <si>
+    <t>17/04/2024 12:17</t>
+  </si>
+  <si>
+    <t>00978457</t>
+  </si>
+  <si>
+    <t>PRISCILA FONSECA DE MOURA</t>
+  </si>
+  <si>
+    <t>19/04/2024 17:21</t>
   </si>
 </sst>
 </file>
@@ -714,11 +750,13 @@
       <sz val="12"/>
       <color rgb="FF56585B"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -807,7 +845,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -852,8 +890,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1168,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,182 +1250,182 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="6">
+        <v>135992</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6">
+        <v>750352</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="6">
+        <v>37001</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="6">
+        <v>37001</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B6" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E6" s="7">
         <v>849960</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="H2" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="H6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B7" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E7" s="7">
         <v>68688</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G7" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="H3" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B8" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E8" s="7">
         <v>68688</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>218</v>
-      </c>
-      <c r="H4" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="7">
-        <v>135992</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="E6" s="7">
-        <v>6776</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="H6" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="E7" s="7">
-        <v>10218</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="H7" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="E8" s="7">
-        <v>9236</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>73</v>
       </c>
       <c r="H8" s="8">
         <v>1</v>
@@ -1396,25 +1433,25 @@
     </row>
     <row r="9" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>195</v>
+        <v>19</v>
       </c>
       <c r="E9" s="7">
-        <v>750352</v>
+        <v>135992</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H9" s="8">
         <v>1</v>
@@ -1422,96 +1459,96 @@
     </row>
     <row r="10" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>15</v>
+        <v>207</v>
       </c>
       <c r="E10" s="7">
-        <v>750352</v>
+        <v>6776</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>157</v>
+        <v>208</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>11</v>
+        <v>209</v>
       </c>
       <c r="H10" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>184</v>
+        <v>199</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>200</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="E11" s="8">
-        <v>158550</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>158</v>
+        <v>202</v>
+      </c>
+      <c r="E11" s="7">
+        <v>10218</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>162</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="H11" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="H11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="8">
-        <v>135992</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>158</v>
+        <v>163</v>
+      </c>
+      <c r="E12" s="7">
+        <v>9236</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>162</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="H12" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="8">
+    <row r="13" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="E13" s="7">
         <v>750352</v>
       </c>
       <c r="F13" s="8" t="s">
@@ -1524,18 +1561,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E14" s="7">
         <v>750352</v>
@@ -1546,187 +1583,187 @@
       <c r="G14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="6">
-        <v>19869</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>159</v>
+      <c r="A15" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E15" s="8">
+        <v>158550</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>158</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="15">
+        <v>187</v>
+      </c>
+      <c r="H15" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="6">
-        <v>26191</v>
+      <c r="A16" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="8">
+        <v>135992</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" s="11">
+        <v>158</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>167</v>
+      <c r="A17" s="6" t="s">
+        <v>178</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>3</v>
+        <v>179</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>4</v>
+        <v>180</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="6">
-        <v>34799</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" s="4">
+        <v>15</v>
+      </c>
+      <c r="E17" s="8">
+        <v>750352</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="A18" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="7">
         <v>750352</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>13</v>
+        <v>173</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>14</v>
+        <v>174</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="E19" s="6">
-        <v>750352</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="4">
+        <v>19869</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>16</v>
+        <v>169</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>18</v>
+        <v>170</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="E20" s="6">
-        <v>135992</v>
+        <v>26191</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="4">
+        <v>69</v>
+      </c>
+      <c r="H20" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>21</v>
+      <c r="A21" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="E21" s="6">
-        <v>47505</v>
+        <v>34799</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>156</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="H21" s="4">
         <v>1</v>
@@ -1734,25 +1771,25 @@
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E22" s="6">
-        <v>19869</v>
+        <v>750352</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H22" s="4">
         <v>1</v>
@@ -1760,16 +1797,16 @@
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E23" s="6">
         <v>750352</v>
@@ -1786,25 +1823,25 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E24" s="6">
-        <v>34799</v>
+        <v>135992</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="H24" s="4">
         <v>1</v>
@@ -1812,25 +1849,25 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="E25" s="6">
-        <v>34799</v>
+        <v>47505</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>156</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="H25" s="4">
         <v>1</v>
@@ -1838,25 +1875,25 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="E26" s="6">
-        <v>34799</v>
+        <v>19869</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="H26" s="4">
         <v>1</v>
@@ -1864,25 +1901,25 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E27" s="6">
-        <v>135992</v>
+        <v>750352</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H27" s="4">
         <v>1</v>
@@ -1890,25 +1927,25 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E28" s="6">
-        <v>58475</v>
+        <v>34799</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>156</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="H28" s="4">
         <v>1</v>
@@ -1916,25 +1953,25 @@
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="E29" s="6">
-        <v>8157</v>
+        <v>34799</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="H29" s="4">
         <v>1</v>
@@ -1942,25 +1979,25 @@
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="E30" s="6">
-        <v>99999</v>
+        <v>34799</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="H30" s="4">
         <v>1</v>
@@ -1968,13 +2005,13 @@
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>19</v>
@@ -1994,25 +2031,25 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="E32" s="6">
-        <v>26191</v>
+        <v>58475</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="H32" s="4">
         <v>1</v>
@@ -2020,25 +2057,25 @@
     </row>
     <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>163</v>
+        <v>55</v>
       </c>
       <c r="E33" s="6">
-        <v>9236</v>
+        <v>8157</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="H33" s="4">
         <v>1</v>
@@ -2046,25 +2083,25 @@
     </row>
     <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E34" s="6">
-        <v>58475</v>
+        <v>99999</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H34" s="4">
         <v>1</v>
@@ -2072,25 +2109,25 @@
     </row>
     <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E35" s="6">
-        <v>19869</v>
+        <v>135992</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H35" s="4">
         <v>1</v>
@@ -2098,25 +2135,25 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="E36" s="6">
-        <v>19869</v>
+        <v>26191</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="H36" s="4">
         <v>1</v>
@@ -2124,25 +2161,25 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>19</v>
+        <v>163</v>
       </c>
       <c r="E37" s="6">
-        <v>135992</v>
+        <v>9236</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="H37" s="4">
         <v>1</v>
@@ -2150,25 +2187,25 @@
     </row>
     <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="E38" s="6">
-        <v>30024</v>
+        <v>58475</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="H38" s="4">
         <v>1</v>
@@ -2176,25 +2213,25 @@
     </row>
     <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E39" s="6">
-        <v>37001</v>
+        <v>19869</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>159</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="H39" s="4">
         <v>1</v>
@@ -2202,25 +2239,25 @@
     </row>
     <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>163</v>
+        <v>29</v>
       </c>
       <c r="E40" s="6">
-        <v>9236</v>
+        <v>19869</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="H40" s="4">
         <v>1</v>
@@ -2228,16 +2265,16 @@
     </row>
     <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="E41" s="6">
         <v>135992</v>
@@ -2254,25 +2291,25 @@
     </row>
     <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="E42" s="6">
-        <v>135992</v>
+        <v>30024</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="H42" s="4">
         <v>1</v>
@@ -2280,25 +2317,25 @@
     </row>
     <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E43" s="6">
-        <v>9939969</v>
+        <v>37001</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="H43" s="4">
         <v>1</v>
@@ -2306,25 +2343,25 @@
     </row>
     <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>10</v>
+        <v>163</v>
       </c>
       <c r="E44" s="6">
-        <v>750352</v>
+        <v>9236</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="H44" s="4">
         <v>1</v>
@@ -2332,25 +2369,25 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="E45" s="6">
-        <v>750352</v>
+        <v>135992</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H45" s="4">
         <v>1</v>
@@ -2358,25 +2395,25 @@
     </row>
     <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E46" s="6">
-        <v>750352</v>
+        <v>135992</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H46" s="4">
         <v>1</v>
@@ -2384,25 +2421,25 @@
     </row>
     <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E47" s="6">
-        <v>750352</v>
+        <v>9939969</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>11</v>
+        <v>108</v>
       </c>
       <c r="H47" s="4">
         <v>1</v>
@@ -2410,13 +2447,13 @@
     </row>
     <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>10</v>
@@ -2436,25 +2473,25 @@
     </row>
     <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E49" s="6">
-        <v>19869</v>
+        <v>750352</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H49" s="4">
         <v>1</v>
@@ -2462,25 +2499,25 @@
     </row>
     <row r="50" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E50" s="6">
-        <v>19869</v>
+        <v>750352</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H50" s="4">
         <v>1</v>
@@ -2488,25 +2525,25 @@
     </row>
     <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E51" s="6">
-        <v>19869</v>
+        <v>750352</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H51" s="4">
         <v>1</v>
@@ -2514,25 +2551,25 @@
     </row>
     <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E52" s="6">
-        <v>37001</v>
+        <v>750352</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="H52" s="4">
         <v>1</v>
@@ -2540,25 +2577,25 @@
     </row>
     <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>163</v>
+        <v>29</v>
       </c>
       <c r="E53" s="6">
-        <v>9236</v>
+        <v>19869</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="H53" s="4">
         <v>1</v>
@@ -2566,25 +2603,25 @@
     </row>
     <row r="54" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="E54" s="6">
-        <v>55450</v>
+        <v>19869</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>142</v>
+        <v>30</v>
       </c>
       <c r="H54" s="4">
         <v>1</v>
@@ -2592,25 +2629,25 @@
     </row>
     <row r="55" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E55" s="6">
-        <v>37001</v>
+        <v>19869</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>159</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="H55" s="4">
         <v>1</v>
@@ -2618,16 +2655,16 @@
     </row>
     <row r="56" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E56" s="6">
         <v>37001</v>
@@ -2644,25 +2681,25 @@
     </row>
     <row r="57" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>50</v>
+        <v>163</v>
       </c>
       <c r="E57" s="6">
-        <v>55450</v>
+        <v>9236</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>142</v>
+        <v>73</v>
       </c>
       <c r="H57" s="4">
         <v>1</v>
@@ -2670,27 +2707,131 @@
     </row>
     <row r="58" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E58" s="6">
+        <v>55450</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H58" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="6">
+        <v>37001</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H59" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E60" s="6">
+        <v>37001</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H60" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E61" s="6">
+        <v>55450</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H61" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D62" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E58" s="6">
+      <c r="E62" s="6">
         <v>750352</v>
       </c>
-      <c r="F58" s="6" t="s">
+      <c r="F62" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="G58" s="1" t="s">
+      <c r="G62" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H58" s="4">
+      <c r="H62" s="4">
         <v>1</v>
       </c>
     </row>
@@ -2698,7 +2839,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:A18 A19:A58" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:A22 A23:A62" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizacao Lista Pacientes Encaminhados Ate o Dia 09-05-2024
</commit_message>
<xml_diff>
--- a/pacientes_imuno_mediados_encaminhados_27_02-2024.xlsx
+++ b/pacientes_imuno_mediados_encaminhados_27_02-2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keller\Documents\Projetos\Cursos\Python\Dashboard_Area_Logada\Area_Logada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD57A93A-CDD5-4D9C-8C01-52BE1607C512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C0C684-A554-410F-BCC9-28D82709DB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Encaminhamento Imuno" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="323">
   <si>
     <t>Número do caso</t>
   </si>
@@ -731,6 +731,264 @@
   </si>
   <si>
     <t>19/04/2024 17:21</t>
+  </si>
+  <si>
+    <t>01006339</t>
+  </si>
+  <si>
+    <t>Thais Fernanda Leite Pinheiro</t>
+  </si>
+  <si>
+    <t>05/05/2024 11:56</t>
+  </si>
+  <si>
+    <t>01005819</t>
+  </si>
+  <si>
+    <t>Isabella Nogueira Silva</t>
+  </si>
+  <si>
+    <t>03/05/2024 17:09</t>
+  </si>
+  <si>
+    <t>01003550</t>
+  </si>
+  <si>
+    <t>AUREA MARIA CAETANO MAIO</t>
+  </si>
+  <si>
+    <t>03/05/2024 09:40</t>
+  </si>
+  <si>
+    <t>Bruno Martins Fernandes Silva</t>
+  </si>
+  <si>
+    <t>01002300</t>
+  </si>
+  <si>
+    <t>Valkiria Canetti Avelar Cerutti</t>
+  </si>
+  <si>
+    <t>02/05/2024 15:55</t>
+  </si>
+  <si>
+    <t>01000050</t>
+  </si>
+  <si>
+    <t>CELIA RODRIGUES DE CARVALHO</t>
+  </si>
+  <si>
+    <t>01/05/2024 20:18</t>
+  </si>
+  <si>
+    <t>Fernanda Oliveira Ferraz</t>
+  </si>
+  <si>
+    <t>00999178</t>
+  </si>
+  <si>
+    <t>Adelina Maria Ferreira Regalado</t>
+  </si>
+  <si>
+    <t>30/04/2024 17:43</t>
+  </si>
+  <si>
+    <t>00997296</t>
+  </si>
+  <si>
+    <t>SILVANIRA DA SILVA MODESTO</t>
+  </si>
+  <si>
+    <t>30/04/2024 11:22</t>
+  </si>
+  <si>
+    <t>00994655</t>
+  </si>
+  <si>
+    <t>Monica Torres Lima Da Silveira</t>
+  </si>
+  <si>
+    <t>29/04/2024 13:01</t>
+  </si>
+  <si>
+    <t>CETTRO - ASA NORTE (EDIFÍCIO DE CLÍNICAS)</t>
+  </si>
+  <si>
+    <t>00994316</t>
+  </si>
+  <si>
+    <t>Juliana Pires de Albuquerque</t>
+  </si>
+  <si>
+    <t>29/04/2024 11:48</t>
+  </si>
+  <si>
+    <t>00994293</t>
+  </si>
+  <si>
+    <t>Juliana Drummond Martins</t>
+  </si>
+  <si>
+    <t>29/04/2024 11:44</t>
+  </si>
+  <si>
+    <t>00994275</t>
+  </si>
+  <si>
+    <t>Jorge Luis Xavier Pereira</t>
+  </si>
+  <si>
+    <t>29/04/2024 11:42</t>
+  </si>
+  <si>
+    <t>00994252</t>
+  </si>
+  <si>
+    <t>Dariane da Silva</t>
+  </si>
+  <si>
+    <t>29/04/2024 11:38</t>
+  </si>
+  <si>
+    <t>ICB - BIOSPHERE (ASA NORTE)</t>
+  </si>
+  <si>
+    <t>00994189</t>
+  </si>
+  <si>
+    <t>VALDENE ARAUJO PICHARA DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>29/04/2024 11:28</t>
+  </si>
+  <si>
+    <t>Imunomed</t>
+  </si>
+  <si>
+    <t>00994052</t>
+  </si>
+  <si>
+    <t>Eugenio Pacelli Rodrigues De Queiroz</t>
+  </si>
+  <si>
+    <t>29/04/2024 11:06</t>
+  </si>
+  <si>
+    <t>00993738</t>
+  </si>
+  <si>
+    <t>Carolina Gomes Da Silva Geraldo</t>
+  </si>
+  <si>
+    <t>29/04/2024 10:17</t>
+  </si>
+  <si>
+    <t>00993702</t>
+  </si>
+  <si>
+    <t>Thayuan Silva Yamada</t>
+  </si>
+  <si>
+    <t>29/04/2024 10:10</t>
+  </si>
+  <si>
+    <t>00993682</t>
+  </si>
+  <si>
+    <t>Ligia Alves de oliveira</t>
+  </si>
+  <si>
+    <t>29/04/2024 10:06</t>
+  </si>
+  <si>
+    <t>00993610</t>
+  </si>
+  <si>
+    <t>Josafa Rodrigues Carvalho Silva</t>
+  </si>
+  <si>
+    <t>29/04/2024 09:57</t>
+  </si>
+  <si>
+    <t>00993525</t>
+  </si>
+  <si>
+    <t>Indira Ramos Gomes</t>
+  </si>
+  <si>
+    <t>29/04/2024 09:41</t>
+  </si>
+  <si>
+    <t>00993496</t>
+  </si>
+  <si>
+    <t>Daniela Cristina Barbosa Da Cruz</t>
+  </si>
+  <si>
+    <t>29/04/2024 09:36</t>
+  </si>
+  <si>
+    <t>00993435</t>
+  </si>
+  <si>
+    <t>CAIO ALVES LEMOS</t>
+  </si>
+  <si>
+    <t>29/04/2024 09:26</t>
+  </si>
+  <si>
+    <t>00993002</t>
+  </si>
+  <si>
+    <t>Isabela Fontinele Costa Freitas</t>
+  </si>
+  <si>
+    <t>28/04/2024 18:59</t>
+  </si>
+  <si>
+    <t>00990914</t>
+  </si>
+  <si>
+    <t>26/04/2024 11:42</t>
+  </si>
+  <si>
+    <t>00989958</t>
+  </si>
+  <si>
+    <t>Ana Helena Peres Correa</t>
+  </si>
+  <si>
+    <t>25/04/2024 19:05</t>
+  </si>
+  <si>
+    <t>00982212</t>
+  </si>
+  <si>
+    <t>Maria Esther Ribera De Vargas</t>
+  </si>
+  <si>
+    <t>23/04/2024 09:56</t>
+  </si>
+  <si>
+    <t>00981426</t>
+  </si>
+  <si>
+    <t>NINA BARAUNA BEZERRA BORGES</t>
+  </si>
+  <si>
+    <t>22/04/2024 16:46</t>
+  </si>
+  <si>
+    <t>00981012</t>
+  </si>
+  <si>
+    <t>Jakeline Wnuk Teixeira</t>
+  </si>
+  <si>
+    <t>22/04/2024 15:17</t>
+  </si>
+  <si>
+    <t>Lucas Leonardo de Castro Borges</t>
   </si>
 </sst>
 </file>
@@ -845,7 +1103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -890,7 +1148,21 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1205,17 +1477,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
     <col min="4" max="4" width="54.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" style="4" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -1249,391 +1521,391 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E2" s="6">
+        <v>19869</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="6">
         <v>135992</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F3" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6">
-        <v>750352</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="E4" s="6">
+        <v>1000918</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="6">
-        <v>37001</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>159</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>94</v>
+        <v>246</v>
       </c>
       <c r="H4" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>226</v>
+        <v>248</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>227</v>
+        <v>249</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E5" s="6">
-        <v>37001</v>
-      </c>
-      <c r="F5" s="8" t="s">
+        <v>19869</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>159</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="H5" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="A6" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="6">
+        <v>25190</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E7" s="6">
         <v>849960</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F7" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G7" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="H6" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="7">
-        <v>68688</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>218</v>
-      </c>
       <c r="H7" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="E8" s="7">
-        <v>68688</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>218</v>
+      <c r="A8" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="6">
+        <v>99999</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="H8" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="7">
-        <v>135992</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>20</v>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E9" s="6">
+        <v>25190</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>253</v>
       </c>
       <c r="H9" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="E10" s="7">
-        <v>6776</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>209</v>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="6">
+        <v>25190</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>253</v>
       </c>
       <c r="H10" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="E11" s="7">
-        <v>10218</v>
-      </c>
-      <c r="F11" s="8" t="s">
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="6">
+        <v>25190</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="6">
+        <v>25190</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E13" s="6">
+        <v>25190</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E14" s="6">
+        <v>9236</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="H11" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="E12" s="7">
-        <v>9236</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="G12" s="9" t="s">
+      <c r="G14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H12" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="E13" s="7">
-        <v>750352</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="7">
-        <v>750352</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="H14" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="E15" s="8">
-        <v>158550</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="H15" s="12">
+      <c r="A15" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="6">
+        <v>25190</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H15" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="8">
-        <v>135992</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>20</v>
+      <c r="A16" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="6">
+        <v>25190</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>253</v>
       </c>
       <c r="H16" s="8">
         <v>1</v>
@@ -1641,831 +1913,831 @@
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>178</v>
+        <v>287</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>179</v>
+        <v>288</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>180</v>
+        <v>289</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="8">
-        <v>750352</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>11</v>
+        <v>55</v>
+      </c>
+      <c r="E17" s="6">
+        <v>25190</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>253</v>
       </c>
       <c r="H17" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="7">
-        <v>750352</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="15">
+      <c r="A18" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="6">
+        <v>25190</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H18" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>172</v>
+        <v>293</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>173</v>
+        <v>294</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>174</v>
+        <v>295</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="E19" s="6">
-        <v>19869</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="15">
+        <v>25190</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H19" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>169</v>
+        <v>296</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>170</v>
+        <v>297</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>171</v>
+        <v>298</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E20" s="6">
-        <v>26191</v>
-      </c>
-      <c r="F20" s="6" t="s">
+        <v>25190</v>
+      </c>
+      <c r="F20" s="16" t="s">
         <v>160</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H20" s="11">
+        <v>253</v>
+      </c>
+      <c r="H20" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>167</v>
+      <c r="A21" s="6" t="s">
+        <v>299</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>4</v>
+        <v>301</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="E21" s="6">
-        <v>34799</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>156</v>
+        <v>25190</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>160</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="4">
+        <v>253</v>
+      </c>
+      <c r="H21" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>8</v>
+        <v>303</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>9</v>
+        <v>304</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E22" s="6">
-        <v>750352</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>157</v>
+        <v>25190</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>160</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="4">
+        <v>253</v>
+      </c>
+      <c r="H22" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>12</v>
+        <v>305</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>13</v>
+        <v>306</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>14</v>
+        <v>307</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="E23" s="6">
-        <v>750352</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>157</v>
+        <v>25190</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>160</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="4">
+        <v>253</v>
+      </c>
+      <c r="H23" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>16</v>
+        <v>308</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>18</v>
+        <v>184</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>309</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E24" s="6">
-        <v>135992</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>158</v>
+        <v>99999</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="4">
+        <v>61</v>
+      </c>
+      <c r="H24" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>21</v>
+        <v>310</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>311</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>23</v>
+        <v>312</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E25" s="6">
-        <v>47505</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>156</v>
+        <v>750352</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H25" s="4">
+        <v>11</v>
+      </c>
+      <c r="H25" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>26</v>
+        <v>313</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>27</v>
+        <v>314</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>28</v>
+        <v>315</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>29</v>
+        <v>280</v>
       </c>
       <c r="E26" s="6">
-        <v>19869</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>159</v>
+        <v>99999</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H26" s="4">
+        <v>61</v>
+      </c>
+      <c r="H26" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>31</v>
+        <v>316</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>317</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>33</v>
+        <v>318</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>10</v>
+        <v>280</v>
       </c>
       <c r="E27" s="6">
-        <v>750352</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>157</v>
+        <v>9236</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>162</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="4">
+        <v>73</v>
+      </c>
+      <c r="H27" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>34</v>
+        <v>319</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>35</v>
+        <v>320</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>36</v>
+        <v>321</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="E28" s="6">
-        <v>34799</v>
-      </c>
-      <c r="F28" s="6" t="s">
+        <v>55314</v>
+      </c>
+      <c r="F28" s="16" t="s">
         <v>156</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H28" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H28" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="17">
+        <v>135992</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="6">
+        <v>750352</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="6">
+        <v>37001</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H31" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="6">
+        <v>37001</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H32" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="7">
+        <v>849960</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="H33" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="6">
-        <v>34799</v>
-      </c>
-      <c r="F29" s="6" t="s">
+      <c r="E34" s="7">
+        <v>68688</v>
+      </c>
+      <c r="F34" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H29" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="6">
-        <v>34799</v>
-      </c>
-      <c r="F30" s="6" t="s">
+      <c r="G34" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="H34" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="E35" s="7">
+        <v>68688</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H30" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="1" t="s">
+      <c r="G35" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="H35" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D36" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E36" s="7">
         <v>135992</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F36" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G36" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E32" s="6">
-        <v>58475</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H32" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E33" s="6">
-        <v>8157</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H33" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E34" s="6">
-        <v>99999</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H34" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="H36" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="E37" s="7">
+        <v>6776</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="H37" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E38" s="7">
+        <v>10218</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="H38" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E39" s="7">
+        <v>9236</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H39" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="E40" s="7">
+        <v>750352</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="7">
+        <v>750352</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E42" s="8">
+        <v>158550</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="H42" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="D43" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E43" s="8">
         <v>135992</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="F43" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G43" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H35" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" s="6">
-        <v>26191</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H36" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E37" s="6">
-        <v>9236</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H37" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E38" s="6">
-        <v>58475</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H38" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E39" s="6">
-        <v>19869</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E40" s="6">
-        <v>19869</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H40" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E41" s="6">
-        <v>135992</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H41" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E42" s="6">
-        <v>30024</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H42" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E43" s="6">
-        <v>37001</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H43" s="4">
+      <c r="H43" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>95</v>
+        <v>178</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>96</v>
+        <v>179</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>97</v>
+        <v>180</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E44" s="6">
-        <v>9236</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H44" s="4">
+        <v>15</v>
+      </c>
+      <c r="E44" s="8">
+        <v>750352</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E45" s="6">
-        <v>135992</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H45" s="4">
+      <c r="A45" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="7">
+        <v>750352</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>102</v>
+        <v>172</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>103</v>
+        <v>173</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>104</v>
+        <v>174</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E46" s="6">
-        <v>135992</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H46" s="4">
+        <v>19869</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H46" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>105</v>
+        <v>169</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>106</v>
+        <v>170</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>107</v>
+        <v>171</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="E47" s="6">
-        <v>9939969</v>
+        <v>26191</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H47" s="4">
+        <v>69</v>
+      </c>
+      <c r="H47" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>109</v>
+      <c r="A48" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>110</v>
+        <v>3</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E48" s="6">
-        <v>750352</v>
+        <v>34799</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H48" s="4">
         <v>1</v>
@@ -2473,13 +2745,13 @@
     </row>
     <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>114</v>
+        <v>9</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>10</v>
@@ -2499,16 +2771,16 @@
     </row>
     <row r="50" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>116</v>
+        <v>13</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>117</v>
+        <v>14</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E50" s="6">
         <v>750352</v>
@@ -2525,25 +2797,25 @@
     </row>
     <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>118</v>
+        <v>16</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>120</v>
+        <v>17</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E51" s="6">
-        <v>750352</v>
+        <v>135992</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H51" s="4">
         <v>1</v>
@@ -2551,25 +2823,25 @@
     </row>
     <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>121</v>
+        <v>21</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>122</v>
+        <v>22</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>123</v>
+        <v>23</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E52" s="6">
-        <v>750352</v>
+        <v>47505</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="H52" s="4">
         <v>1</v>
@@ -2577,13 +2849,13 @@
     </row>
     <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>124</v>
+        <v>26</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>125</v>
+        <v>27</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>29</v>
@@ -2603,25 +2875,25 @@
     </row>
     <row r="54" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>127</v>
+        <v>31</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>129</v>
+        <v>33</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E54" s="6">
-        <v>19869</v>
+        <v>750352</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H54" s="4">
         <v>1</v>
@@ -2629,25 +2901,25 @@
     </row>
     <row r="55" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>130</v>
+        <v>34</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>131</v>
+        <v>35</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>132</v>
+        <v>36</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E55" s="6">
-        <v>19869</v>
+        <v>34799</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="H55" s="4">
         <v>1</v>
@@ -2655,25 +2927,25 @@
     </row>
     <row r="56" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>133</v>
+        <v>38</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>134</v>
+        <v>39</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>135</v>
+        <v>40</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E56" s="6">
-        <v>37001</v>
+        <v>34799</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>94</v>
+        <v>6</v>
       </c>
       <c r="H56" s="4">
         <v>1</v>
@@ -2681,25 +2953,25 @@
     </row>
     <row r="57" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>136</v>
+        <v>41</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>137</v>
+        <v>42</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>138</v>
+        <v>43</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>163</v>
+        <v>5</v>
       </c>
       <c r="E57" s="6">
-        <v>9236</v>
+        <v>34799</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="H57" s="4">
         <v>1</v>
@@ -2707,25 +2979,25 @@
     </row>
     <row r="58" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>139</v>
+        <v>44</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>140</v>
+        <v>45</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>141</v>
+        <v>46</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="E58" s="6">
-        <v>55450</v>
+        <v>135992</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>142</v>
+        <v>20</v>
       </c>
       <c r="H58" s="4">
         <v>1</v>
@@ -2733,25 +3005,25 @@
     </row>
     <row r="59" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>143</v>
+        <v>47</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>144</v>
+        <v>48</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>145</v>
+        <v>49</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="E59" s="6">
-        <v>37001</v>
+        <v>58475</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="H59" s="4">
         <v>1</v>
@@ -2759,25 +3031,25 @@
     </row>
     <row r="60" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>146</v>
+        <v>52</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>147</v>
+        <v>53</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>148</v>
+        <v>54</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="E60" s="6">
-        <v>37001</v>
+        <v>8157</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="H60" s="4">
         <v>1</v>
@@ -2785,25 +3057,25 @@
     </row>
     <row r="61" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>149</v>
+        <v>57</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>150</v>
+        <v>58</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>151</v>
+        <v>59</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E61" s="6">
-        <v>55450</v>
+        <v>99999</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>142</v>
+        <v>61</v>
       </c>
       <c r="H61" s="4">
         <v>1</v>
@@ -2811,27 +3083,729 @@
     </row>
     <row r="62" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" s="6">
+        <v>135992</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H62" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E63" s="6">
+        <v>26191</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H63" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E64" s="6">
+        <v>9236</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H64" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E65" s="6">
+        <v>58475</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H65" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E66" s="6">
+        <v>19869</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H66" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E67" s="6">
+        <v>19869</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H67" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E68" s="6">
+        <v>135992</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H68" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E69" s="6">
+        <v>30024</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H69" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E70" s="6">
+        <v>37001</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H70" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E71" s="6">
+        <v>9236</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H71" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E72" s="6">
+        <v>135992</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H72" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E73" s="6">
+        <v>135992</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H73" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" s="6">
+        <v>9939969</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H74" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="6">
+        <v>750352</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H75" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="6">
+        <v>750352</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H76" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="6">
+        <v>750352</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H77" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" s="6">
+        <v>750352</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H78" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="6">
+        <v>750352</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H79" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E80" s="6">
+        <v>19869</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H80" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E81" s="6">
+        <v>19869</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H81" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E82" s="6">
+        <v>19869</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H82" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E83" s="6">
+        <v>37001</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H83" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E84" s="6">
+        <v>9236</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H84" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E85" s="6">
+        <v>55450</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H85" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E86" s="6">
+        <v>37001</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H86" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E87" s="6">
+        <v>37001</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H87" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E88" s="6">
+        <v>55450</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H88" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D89" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E62" s="6">
+      <c r="E89" s="6">
         <v>750352</v>
       </c>
-      <c r="F62" s="6" t="s">
+      <c r="F89" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="G62" s="1" t="s">
+      <c r="G89" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H62" s="4">
+      <c r="H89" s="4">
         <v>1</v>
       </c>
     </row>
@@ -2839,7 +3813,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:A22 A23:A62" numberStoredAsText="1"/>
+    <ignoredError sqref="A29:A49 A50:A89 A2:A28" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizacao Lista Pacientes Encaminhados Excluindo os Testes
</commit_message>
<xml_diff>
--- a/pacientes_imuno_mediados_encaminhados_27_02-2024.xlsx
+++ b/pacientes_imuno_mediados_encaminhados_27_02-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keller\Documents\Projetos\Cursos\Python\Dashboard_Area_Logada\Area_Logada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7792A8-0E51-42D4-B213-7240D65E1CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E01E52E-D046-47CC-BBE6-E7365045F407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1760,7 +1760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1835,14 +1835,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2162,7 +2155,7 @@
   <dimension ref="A1:H156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H141" sqref="H141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2203,8 +2196,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
         <v>507</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2219,7 +2212,7 @@
       <c r="E2" s="6">
         <v>12003</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="8" t="s">
         <v>160</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -2229,8 +2222,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>508</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2245,7 +2238,7 @@
       <c r="E3" s="6">
         <v>478659</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="8" t="s">
         <v>157</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -2255,8 +2248,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
         <v>509</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2271,7 +2264,7 @@
       <c r="E4" s="6">
         <v>750352</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="8" t="s">
         <v>157</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -2281,8 +2274,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
         <v>510</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2297,7 +2290,7 @@
       <c r="E5" s="6">
         <v>24195</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="8" t="s">
         <v>160</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -2307,8 +2300,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
         <v>511</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2323,7 +2316,7 @@
       <c r="E6" s="6">
         <v>25190</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="8" t="s">
         <v>160</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -2334,7 +2327,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="26" t="s">
         <v>512</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2360,7 +2353,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="26" t="s">
         <v>513</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2386,7 +2379,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="26" t="s">
         <v>514</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2408,11 +2401,11 @@
         <v>61</v>
       </c>
       <c r="H9" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="26" t="s">
         <v>515</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2438,7 +2431,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="26" t="s">
         <v>516</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2464,7 +2457,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="26" t="s">
         <v>517</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2490,7 +2483,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="26" t="s">
         <v>518</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2516,7 +2509,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="26" t="s">
         <v>519</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2542,7 +2535,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="26" t="s">
         <v>520</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2568,7 +2561,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="26" t="s">
         <v>521</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -2594,7 +2587,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="26" t="s">
         <v>522</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2620,7 +2613,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="26" t="s">
         <v>523</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2646,7 +2639,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="26" t="s">
         <v>524</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2672,7 +2665,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="26" t="s">
         <v>525</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2698,7 +2691,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="26" t="s">
         <v>526</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2724,7 +2717,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="26" t="s">
         <v>527</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -3136,7 +3129,7 @@
         <v>187</v>
       </c>
       <c r="H37" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3500,7 +3493,7 @@
         <v>187</v>
       </c>
       <c r="H51" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3526,7 +3519,7 @@
         <v>187</v>
       </c>
       <c r="H52" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4124,7 +4117,7 @@
         <v>61</v>
       </c>
       <c r="H75" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4540,7 +4533,7 @@
         <v>61</v>
       </c>
       <c r="H91" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4592,7 +4585,7 @@
         <v>61</v>
       </c>
       <c r="H93" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -5008,7 +5001,7 @@
         <v>187</v>
       </c>
       <c r="H109" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -5502,7 +5495,7 @@
         <v>61</v>
       </c>
       <c r="H128" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -5840,7 +5833,7 @@
         <v>108</v>
       </c>
       <c r="H141" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Atualizacao Lista Pacientes Encaminhados Ate o Dia 08/10/2024 - Arquivo Sem Marcadores de Cor
</commit_message>
<xml_diff>
--- a/pacientes_imuno_mediados_encaminhados_27_02-2024.xlsx
+++ b/pacientes_imuno_mediados_encaminhados_27_02-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keller\Documents\Projetos\Cursos\Python\Dashboard_Area_Logada\Area_Logada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094D2669-F99D-4DCB-88F4-BE80A68DCA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70ACE01-3979-4217-9917-6AF51153F241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2735,7 +2735,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2750,12 +2750,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2864,22 +2858,22 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3194,10 +3188,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3732,7 +3727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
         <v>650</v>
       </c>
@@ -3758,7 +3753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
         <v>651</v>
       </c>
@@ -4044,7 +4039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
         <v>662</v>
       </c>
@@ -4512,7 +4507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="26" t="s">
         <v>680</v>
       </c>
@@ -6176,7 +6171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="26" t="s">
         <v>514</v>
       </c>
@@ -6904,7 +6899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="22" t="s">
         <v>370</v>
       </c>
@@ -7268,7 +7263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="22" t="s">
         <v>413</v>
       </c>
@@ -7294,7 +7289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="22" t="s">
         <v>416</v>
       </c>
@@ -7892,7 +7887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="6" t="s">
         <v>257</v>
       </c>
@@ -8308,7 +8303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="6" t="s">
         <v>307</v>
       </c>
@@ -8360,7 +8355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="6" t="s">
         <v>312</v>
       </c>
@@ -8776,7 +8771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="7" t="s">
         <v>188</v>
       </c>
@@ -9270,7 +9265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="6" t="s">
         <v>57</v>
       </c>
@@ -9608,7 +9603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="6" t="s">
         <v>105</v>
       </c>
@@ -10025,6 +10020,56 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H262" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="Aedra Kapitzky Dias"/>
+        <filter val="Aline Rocha Camporez"/>
+        <filter val="Anber Ancel Tanaka"/>
+        <filter val="Breno Cesar De Oliveira Viana"/>
+        <filter val="Bruno Martins Fernandes Silva"/>
+        <filter val="Camila Cuzzuol Pimentel Modenese Lima"/>
+        <filter val="Camila da Silva Cendon Duran"/>
+        <filter val="Carolina Moreno Cossi"/>
+        <filter val="Cecilia Resende Brunow Bazzo"/>
+        <filter val="Ernane Pires Maciel"/>
+        <filter val="Fabricio Claudino Estrela Terra Theodoro"/>
+        <filter val="Fernanda Calil Netto Souza"/>
+        <filter val="Fernanda Oliveira Ferraz"/>
+        <filter val="Fernando do Espirito Santo Soares"/>
+        <filter val="Gesmar Rodrigues Silva Segundo"/>
+        <filter val="Gina Eliane Menezes Haase Lobo"/>
+        <filter val="Guilherme Sciascia do Olival"/>
+        <filter val="Gustavo Pafume de Sa"/>
+        <filter val="Gutemberg Augusto Cruz dos Santos"/>
+        <filter val="Hamilton Cirne Fernandes Franco"/>
+        <filter val="Henry Koiti Sato"/>
+        <filter val="Iracema Ferreira Sanders"/>
+        <filter val="Livia Maria de Oliveira Lopes Costa"/>
+        <filter val="Lucas Leonardo de Castro Borges"/>
+        <filter val="Luma Alem Martins"/>
+        <filter val="Marcos Milanesi Lofrano"/>
+        <filter val="Marcos Papais Alvarenga"/>
+        <filter val="Matheus Pedro Wasem"/>
+        <filter val="Mayara Manueira da Silveira"/>
+        <filter val="Milton da Silveira Pedreira Neto"/>
+        <filter val="Natalia Nasser Ximenes"/>
+        <filter val="Natalia Solon Nery"/>
+        <filter val="Patricia Mayumi Kurihara"/>
+        <filter val="Paulo Antonio Oldani Felix"/>
+        <filter val="Paulo Eduardo Silva Belluco"/>
+        <filter val="Pedro Dantas Oliveira"/>
+        <filter val="Rafael Melo De Deus"/>
+        <filter val="Raquel Vassao Araujo"/>
+        <filter val="Renato de Lima Azambuja"/>
+        <filter val="Ronaldo Maciel Dias"/>
+        <filter val="Sasha Rubim Rocha Bender"/>
+        <filter val="Thales Henrique Viana Azevedo"/>
+        <filter val="Thiago Santos Nascimento"/>
+        <filter val="Wilson Marques Ramos Junior"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>